<commit_message>
ExcelFormulaContext added and findCell updated
</commit_message>
<xml_diff>
--- a/examples/ExcelFormulaParser.Expressions.Console/Book.xlsx
+++ b/examples/ExcelFormulaParser.Expressions.Console/Book.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -440,14 +441,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>POWER(2, 5)+8+Sheet3!A1</f>
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <f>POWER(2, 5)+8+(10/5)</f>
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor + fix range
</commit_message>
<xml_diff>
--- a/examples/ExcelFormulaParser.Expressions.Console/Book.xlsx
+++ b/examples/ExcelFormulaParser.Expressions.Console/Book.xlsx
@@ -400,9 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -427,6 +425,10 @@
       <c r="B2">
         <v>2</v>
       </c>
+      <c r="C2">
+        <f>5*5</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -436,6 +438,9 @@
         <f>B1+B2</f>
         <v>3</v>
       </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -476,8 +481,8 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <f>SUM(B1:C2, 1000)</f>
-        <v>1007</v>
+        <f>SUM(B1:C3, 1000)</f>
+        <v>1034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes and more functions
</commit_message>
<xml_diff>
--- a/examples/ExcelFormulaParser.Expressions.Console/Book.xlsx
+++ b/examples/ExcelFormulaParser.Expressions.Console/Book.xlsx
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="named_range_01">Sheet1!$B$10</definedName>
+    <definedName name="named_range_02">Sheet1!$B$11</definedName>
   </definedNames>
   <calcPr calcId="171027" calcOnSave="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>column a, row 1</t>
   </si>
@@ -68,7 +69,10 @@
     <t>vlookup date</t>
   </si>
   <si>
-    <t>namedrange</t>
+    <t>namedrange2</t>
+  </si>
+  <si>
+    <t>namedrange1</t>
   </si>
 </sst>
 </file>
@@ -426,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +538,7 @@
       </c>
       <c r="B9" s="2">
         <f ca="1">NOW()</f>
-        <v>42899.903908333334</v>
+        <v>42903.456415624998</v>
       </c>
       <c r="C9">
         <f ca="1">MONTH(B9)</f>
@@ -543,11 +547,20 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <f>ROUND(7/9,2)</f>
         <v>0.78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <f>named_range_01+1</f>
+        <v>1.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>